<commit_message>
updates on BOM, CPL and gerbers
</commit_message>
<xml_diff>
--- a/BOM/GPS_MODULE_V3_BOM.xlsx
+++ b/BOM/GPS_MODULE_V3_BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10" conformance="strict">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\kicad6\KICAD 6.0.0\contractual_projects\ECO_BODA\GPS_BAORD\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{99EA318B-A378-4E57-A5F2-AE573DBB6D42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{65DF5049-696E-4F7E-B13A-66B567588E1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="34665" yWindow="4515" windowWidth="13830" windowHeight="8445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
   </bookViews>
   <sheets>
     <sheet name="GPS_MODULE_V3.kicad_pro" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="328" uniqueCount="203">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="313" uniqueCount="197">
   <si>
     <t>Qty</t>
   </si>
@@ -42,6 +42,9 @@
     <t>MPN</t>
   </si>
   <si>
+    <t>AE1, AE2</t>
+  </si>
+  <si>
     <t>Antenna_Shield</t>
   </si>
   <si>
@@ -72,27 +75,39 @@
     <t>33p</t>
   </si>
   <si>
+    <t>C4, C20</t>
+  </si>
+  <si>
+    <t>1u</t>
+  </si>
+  <si>
     <t>C5</t>
   </si>
   <si>
     <t>22u</t>
   </si>
   <si>
+    <t>C6, C16</t>
+  </si>
+  <si>
     <t>10u</t>
   </si>
   <si>
+    <t>C7, C8, C9, C10, C21, C22, C23</t>
+  </si>
+  <si>
     <t>22p</t>
   </si>
   <si>
+    <t>C11, C18, C31</t>
+  </si>
+  <si>
+    <t>C12, C13, C14, C15, C17, C29, C30, C32, C33, C37</t>
+  </si>
+  <si>
     <t>100n</t>
   </si>
   <si>
-    <t>1u</t>
-  </si>
-  <si>
-    <t>C25</t>
-  </si>
-  <si>
     <t>100u</t>
   </si>
   <si>
@@ -102,19 +117,13 @@
     <t>TLJA107M006R0800</t>
   </si>
   <si>
-    <t>C26</t>
-  </si>
-  <si>
-    <t>0.3p</t>
-  </si>
-  <si>
-    <t>C35</t>
-  </si>
-  <si>
-    <t>C36</t>
-  </si>
-  <si>
-    <t>1n</t>
+    <t>C24, C26, C28</t>
+  </si>
+  <si>
+    <t>0.1u</t>
+  </si>
+  <si>
+    <t>C25, C27, C34</t>
   </si>
   <si>
     <t>C38</t>
@@ -129,6 +138,9 @@
     <t>Diode_SMD:D_SOD-123</t>
   </si>
   <si>
+    <t>D2, D3, D4</t>
+  </si>
+  <si>
     <t>SS310</t>
   </si>
   <si>
@@ -147,33 +159,33 @@
     <t>D6</t>
   </si>
   <si>
+    <t>LXES15AAA1-153</t>
+  </si>
+  <si>
+    <t>Diode_SMD:D_0402_1005Metric</t>
+  </si>
+  <si>
+    <t>D7</t>
+  </si>
+  <si>
     <t>SP0504BAHT</t>
   </si>
   <si>
     <t>Package_TO_SOT_SMD:SOT-23-5</t>
   </si>
   <si>
-    <t>D7</t>
+    <t>D8</t>
   </si>
   <si>
     <t>ORANGE</t>
   </si>
   <si>
-    <t>D8</t>
+    <t>D9</t>
   </si>
   <si>
     <t>BLUE</t>
   </si>
   <si>
-    <t>D9</t>
-  </si>
-  <si>
-    <t>LXES15AAA1-153</t>
-  </si>
-  <si>
-    <t>Diode_SMD:D_0402_1005Metric</t>
-  </si>
-  <si>
     <t>D10</t>
   </si>
   <si>
@@ -183,18 +195,12 @@
     <t>Package_TO_SOT_SMD:SOT-23</t>
   </si>
   <si>
+    <t>D11, D12</t>
+  </si>
+  <si>
     <t>BEP0080MA</t>
   </si>
   <si>
-    <t>FL1</t>
-  </si>
-  <si>
-    <t>B39162B8813P810</t>
-  </si>
-  <si>
-    <t>Filter:Filter_1109-5_1.1x0.9mm</t>
-  </si>
-  <si>
     <t>J1</t>
   </si>
   <si>
@@ -207,10 +213,10 @@
     <t>J2</t>
   </si>
   <si>
-    <t>Conn_02x02_Odd_Even</t>
-  </si>
-  <si>
-    <t>Connector_Molex:Molex_Nano-Fit_105314-xx04_2x02_P2.50mm_Horizontal</t>
+    <t>Conn_02x04_Odd_Even</t>
+  </si>
+  <si>
+    <t>Connector_Molex:Molex_Mini-Fit_Jr_5569-08A2_2x04_P4.20mm_Horizontal</t>
   </si>
   <si>
     <t>J3</t>
@@ -225,13 +231,13 @@
     <t>NSIM-2-C</t>
   </si>
   <si>
-    <t>J5</t>
-  </si>
-  <si>
-    <t>Conn_02x03_Odd_Even</t>
-  </si>
-  <si>
-    <t>Connector_Molex:Molex_Nano-Fit_105314-xx06_2x03_P2.50mm_Horizontal</t>
+    <t>J4</t>
+  </si>
+  <si>
+    <t>Micro_SD_Card</t>
+  </si>
+  <si>
+    <t>MACHADA_footprints:MOLEX_503398-1892</t>
   </si>
   <si>
     <t>L1</t>
@@ -258,36 +264,33 @@
     <t>L3</t>
   </si>
   <si>
-    <t>1uH</t>
+    <t>82nH</t>
   </si>
   <si>
     <t>Inductor_SMD:L_0402_1005Metric</t>
   </si>
   <si>
-    <t>L4</t>
-  </si>
-  <si>
-    <t>27nH</t>
-  </si>
-  <si>
-    <t>L5</t>
-  </si>
-  <si>
-    <t>100mHz 150/200R</t>
-  </si>
-  <si>
     <t>Q1</t>
   </si>
   <si>
     <t>SSM3J328R-HXY</t>
   </si>
   <si>
+    <t>Q2, Q3</t>
+  </si>
+  <si>
     <t>BSN20</t>
   </si>
   <si>
+    <t>Q4, Q5, Q6, Q7</t>
+  </si>
+  <si>
     <t>2N7002</t>
   </si>
   <si>
+    <t>R1, R33, R36, R45, R50</t>
+  </si>
+  <si>
     <t>1K</t>
   </si>
   <si>
@@ -315,6 +318,9 @@
     <t>SCR0603F40K</t>
   </si>
   <si>
+    <t>R4, R6, R23, R24</t>
+  </si>
+  <si>
     <t>100K</t>
   </si>
   <si>
@@ -330,37 +336,73 @@
     <t>499R</t>
   </si>
   <si>
+    <t>R8, R30, R31, R34, R35, R43, R44, R48, R49</t>
+  </si>
+  <si>
     <t>10K</t>
   </si>
   <si>
+    <t>R9, R12, R13</t>
+  </si>
+  <si>
     <t>1k</t>
   </si>
   <si>
+    <t>R10, R11, R14</t>
+  </si>
+  <si>
+    <t>R15, R16</t>
+  </si>
+  <si>
+    <t>2.2K</t>
+  </si>
+  <si>
+    <t>R17, R18, R19</t>
+  </si>
+  <si>
     <t>22R</t>
   </si>
   <si>
-    <t>2.2K</t>
-  </si>
-  <si>
-    <t>R19</t>
+    <t>R20</t>
+  </si>
+  <si>
+    <t>200K</t>
+  </si>
+  <si>
+    <t>R21</t>
+  </si>
+  <si>
+    <t>R22, R29</t>
+  </si>
+  <si>
+    <t>390R</t>
+  </si>
+  <si>
+    <t>R25, R26</t>
+  </si>
+  <si>
+    <t>10R</t>
+  </si>
+  <si>
+    <t>R27</t>
+  </si>
+  <si>
+    <t>220R</t>
+  </si>
+  <si>
+    <t>R28, R32</t>
   </si>
   <si>
     <t>0R</t>
   </si>
   <si>
-    <t>R20</t>
-  </si>
-  <si>
-    <t>10R</t>
-  </si>
-  <si>
-    <t>390R</t>
-  </si>
-  <si>
-    <t>R27</t>
-  </si>
-  <si>
-    <t>220R</t>
+    <t>R37, R38, R39, R40, R41, R42</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>R46, R47</t>
   </si>
   <si>
     <t>60R</t>
@@ -396,10 +438,10 @@
     <t>U3</t>
   </si>
   <si>
-    <t>SIM7000E</t>
-  </si>
-  <si>
-    <t>Lib:SIMCON_SIM7000E</t>
+    <t>A9G_MODULE</t>
+  </si>
+  <si>
+    <t>MACHADA_footprints:A9G_MODULE</t>
   </si>
   <si>
     <t>U4</t>
@@ -411,6 +453,15 @@
     <t>Package_SO:SOP-8_3.9x4.9mm_P1.27mm</t>
   </si>
   <si>
+    <t>U5</t>
+  </si>
+  <si>
+    <t>XC6206PxxxMR</t>
+  </si>
+  <si>
+    <t>Package_TO_SOT_SMD:SOT-23-3</t>
+  </si>
+  <si>
     <t>U7</t>
   </si>
   <si>
@@ -447,72 +498,6 @@
     <t>Crystal:Crystal_SMD_3215-2Pin_3.2x1.5mm</t>
   </si>
   <si>
-    <t>AE1, AE2</t>
-  </si>
-  <si>
-    <t>C6, C16</t>
-  </si>
-  <si>
-    <t>C7, C8, C9, C10, C18, C19, C20</t>
-  </si>
-  <si>
-    <t>C12, C13, C14, C15, C17, C21, C29, C30, C32, C33, C37</t>
-  </si>
-  <si>
-    <t>C22, C34</t>
-  </si>
-  <si>
-    <t>C23, C24, C31</t>
-  </si>
-  <si>
-    <t>C27, C28</t>
-  </si>
-  <si>
-    <t>D2, D3, D4</t>
-  </si>
-  <si>
-    <t>D11, D12</t>
-  </si>
-  <si>
-    <t>Q2, Q3</t>
-  </si>
-  <si>
-    <t>Q5, Q6, Q7, Q8, Q9</t>
-  </si>
-  <si>
-    <t>R1, R29, R30, R31, R40, R41</t>
-  </si>
-  <si>
-    <t>R4, R6, R23, R24</t>
-  </si>
-  <si>
-    <t>R8, R33, R34, R35, R37, R38, R39, R42, R43, R44, R45</t>
-  </si>
-  <si>
-    <t>R9, R10</t>
-  </si>
-  <si>
-    <t>R11, R12, R16</t>
-  </si>
-  <si>
-    <t>R13, R14, R15</t>
-  </si>
-  <si>
-    <t>R17, R18</t>
-  </si>
-  <si>
-    <t>R21, R22</t>
-  </si>
-  <si>
-    <t>R25, R26</t>
-  </si>
-  <si>
-    <t>R28, R32</t>
-  </si>
-  <si>
-    <t>R46, R47</t>
-  </si>
-  <si>
     <t>Vendor</t>
   </si>
   <si>
@@ -522,15 +507,15 @@
     <t>0402CG8R2C500NT</t>
   </si>
   <si>
-    <t>CC0402KRX7R9BB103</t>
-  </si>
-  <si>
     <t>CC0603KRX7R9BB103</t>
   </si>
   <si>
     <t>CC0603JRNPO9BN330</t>
   </si>
   <si>
+    <t>CL05A105KP5NNNC</t>
+  </si>
+  <si>
     <t>CL10A226MQ8NRNC</t>
   </si>
   <si>
@@ -540,19 +525,13 @@
     <t>0402CG220J500NT</t>
   </si>
   <si>
+    <t>CL05A106MQ5NUNC</t>
+  </si>
+  <si>
     <t>CC0402KRX7R7BB104</t>
   </si>
   <si>
-    <t>CL05A105KP5NNNC</t>
-  </si>
-  <si>
-    <t>CL05A106MQ5NUNC</t>
-  </si>
-  <si>
-    <t>V0R3B0402C0G500NBT</t>
-  </si>
-  <si>
-    <t>CC0402KRX7R9BB102</t>
+    <t>C36, C39</t>
   </si>
   <si>
     <t>0603B104K500NT</t>
@@ -561,25 +540,19 @@
     <t>XL-1608SURC-06FJ</t>
   </si>
   <si>
-    <t>SP0504BAHTG</t>
-  </si>
-  <si>
     <t>XL-1608UOC-06FJ</t>
   </si>
   <si>
     <t>LTST-C191TBKT</t>
   </si>
   <si>
+    <t>DIGIKEY</t>
+  </si>
+  <si>
     <t>BLM18BD421SH1D</t>
   </si>
   <si>
-    <t>SDFL1005Q1R0KTF</t>
-  </si>
-  <si>
-    <t>LQG15HS27NJ02D</t>
-  </si>
-  <si>
-    <t>CBG160808U201T</t>
+    <t>SDCL1005C82NJTDF</t>
   </si>
   <si>
     <t>RC0402FR-7W1KL</t>
@@ -597,31 +570,40 @@
     <t>RC0402FR-0710KL</t>
   </si>
   <si>
+    <t>RC0603JR-072K2L</t>
+  </si>
+  <si>
     <t>RC0402FR-0722RL</t>
   </si>
   <si>
-    <t>RC0603JR-072K2L</t>
+    <t>0402WGF2003TCE</t>
+  </si>
+  <si>
+    <t>RC0402FR-07390RL</t>
+  </si>
+  <si>
+    <t>0402WGJ0100TCE</t>
+  </si>
+  <si>
+    <t>0402WGF2200TCE</t>
   </si>
   <si>
     <t>0402WGJ0000TCE</t>
   </si>
   <si>
-    <t>0402WGJ0100TCE</t>
-  </si>
-  <si>
-    <t>RC0402FR-07390RL</t>
-  </si>
-  <si>
-    <t>0402WGF2200TCE</t>
-  </si>
-  <si>
     <t>RC0402FR-0760R4L</t>
   </si>
   <si>
     <t>STM32F103C8T6TR</t>
   </si>
   <si>
+    <t>A9G</t>
+  </si>
+  <si>
     <t>MAX485ESA</t>
+  </si>
+  <si>
+    <t>XC6206P282MR</t>
   </si>
   <si>
     <t>W25Q32JVSSIQ</t>
@@ -639,7 +621,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1483,20 +1465,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F66"/>
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.5546875" customWidth="1"/>
-    <col min="2" max="2" width="15.109375" customWidth="1"/>
-    <col min="3" max="3" width="37.44140625" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" customWidth="1"/>
+    <col min="3" max="3" width="47" customWidth="1"/>
+    <col min="4" max="5" width="21.21875" customWidth="1"/>
+    <col min="6" max="6" width="8.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -1513,7 +1495,7 @@
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>0</v>
@@ -1521,19 +1503,19 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>140</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="E2" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F2">
         <v>2</v>
@@ -1541,19 +1523,19 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E3" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -1561,19 +1543,19 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="E4" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -1581,19 +1563,19 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
         <v>13</v>
       </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
       <c r="D5" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="E5" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -1601,139 +1583,139 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="E6" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>141</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="E7" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F7">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>142</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="E8" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F8">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>143</v>
+        <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="E9" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F9">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>144</v>
+        <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="E10" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F10">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>145</v>
+        <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="C11" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="E11" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F11">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>168</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D12" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E12" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F12">
         <v>1</v>
@@ -1741,59 +1723,59 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="C13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>174</v>
+        <v>10</v>
+      </c>
+      <c r="D13" t="s">
+        <v>167</v>
       </c>
       <c r="E13" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F13">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>146</v>
+        <v>32</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="C14" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>174</v>
+        <v>10</v>
+      </c>
+      <c r="D14" t="s">
+        <v>162</v>
       </c>
       <c r="E14" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F14">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="B15" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="C15" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D15" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="E15" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F15">
         <v>1</v>
@@ -1801,19 +1783,19 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" t="s">
-        <v>175</v>
+        <v>36</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="E16" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F16">
         <v>1</v>
@@ -1821,39 +1803,39 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="C17" t="s">
-        <v>12</v>
-      </c>
-      <c r="D17" t="s">
-        <v>176</v>
+        <v>39</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="E17" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F17">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="B18" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C18" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>32</v>
+        <v>170</v>
       </c>
       <c r="E18" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F18">
         <v>1</v>
@@ -1861,39 +1843,39 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>147</v>
+        <v>43</v>
       </c>
       <c r="B19" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="C19" t="s">
-        <v>35</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>34</v>
+        <v>45</v>
+      </c>
+      <c r="D19" t="s">
+        <v>44</v>
       </c>
       <c r="E19" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F19">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="B20" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="C20" t="s">
-        <v>38</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>177</v>
+        <v>48</v>
+      </c>
+      <c r="D20" t="s">
+        <v>47</v>
       </c>
       <c r="E20" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F20">
         <v>1</v>
@@ -1901,19 +1883,19 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="B21" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="C21" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="E21" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F21">
         <v>1</v>
@@ -1921,19 +1903,19 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" t="s">
         <v>42</v>
       </c>
-      <c r="B22" t="s">
-        <v>43</v>
-      </c>
-      <c r="C22" t="s">
-        <v>38</v>
-      </c>
       <c r="D22" s="2" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="E22" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F22">
         <v>1</v>
@@ -1941,19 +1923,19 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="B23" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="C23" t="s">
-        <v>38</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>180</v>
+        <v>55</v>
+      </c>
+      <c r="D23" t="s">
+        <v>54</v>
       </c>
       <c r="E23" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F23">
         <v>1</v>
@@ -1961,39 +1943,39 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="B24" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="C24" t="s">
-        <v>48</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
+      </c>
+      <c r="D24" t="s">
+        <v>57</v>
       </c>
       <c r="E24" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F24">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="B25" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="C25" t="s">
-        <v>51</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>50</v>
+        <v>60</v>
+      </c>
+      <c r="D25" s="2">
+        <v>1751248</v>
       </c>
       <c r="E25" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F25">
         <v>1</v>
@@ -2001,39 +1983,39 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>148</v>
+        <v>61</v>
       </c>
       <c r="B26" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="C26" t="s">
-        <v>33</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>52</v>
+        <v>63</v>
+      </c>
+      <c r="D26" s="2">
+        <v>1053142204</v>
       </c>
       <c r="E26" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F26">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="B27" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="C27" t="s">
-        <v>55</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>54</v>
+        <v>66</v>
+      </c>
+      <c r="D27" t="s">
+        <v>67</v>
       </c>
       <c r="E27" t="s">
-        <v>202</v>
+        <v>173</v>
       </c>
       <c r="F27">
         <v>1</v>
@@ -2041,19 +2023,19 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="B28" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="C28" t="s">
-        <v>58</v>
-      </c>
-      <c r="D28" s="2">
-        <v>1751248</v>
+        <v>70</v>
+      </c>
+      <c r="D28">
+        <v>5033981892</v>
       </c>
       <c r="E28" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F28">
         <v>1</v>
@@ -2061,19 +2043,19 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="B29" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="C29" t="s">
-        <v>61</v>
-      </c>
-      <c r="D29" s="2">
-        <v>1053142204</v>
+        <v>73</v>
+      </c>
+      <c r="D29" t="s">
+        <v>74</v>
       </c>
       <c r="E29" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F29">
         <v>1</v>
@@ -2081,19 +2063,19 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="B30" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="C30" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>65</v>
+        <v>174</v>
       </c>
       <c r="E30" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F30">
         <v>1</v>
@@ -2101,19 +2083,19 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="B31" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C31" t="s">
-        <v>68</v>
-      </c>
-      <c r="D31" s="2">
-        <v>1053142206</v>
+        <v>80</v>
+      </c>
+      <c r="D31" t="s">
+        <v>175</v>
       </c>
       <c r="E31" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F31">
         <v>1</v>
@@ -2121,19 +2103,19 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="B32" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="C32" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="D32" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="E32" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F32">
         <v>1</v>
@@ -2141,79 +2123,79 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="B33" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="C33" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>181</v>
+        <v>84</v>
       </c>
       <c r="E33" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F33">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="B34" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="C34" t="s">
-        <v>78</v>
+        <v>55</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>182</v>
+        <v>86</v>
       </c>
       <c r="E34" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F34">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="B35" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="C35" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="E35" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F35">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="B36" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="C36" t="s">
-        <v>78</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>184</v>
+        <v>89</v>
+      </c>
+      <c r="D36" t="s">
+        <v>92</v>
       </c>
       <c r="E36" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F36">
         <v>1</v>
@@ -2221,19 +2203,19 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="B37" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="C37" t="s">
-        <v>51</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>84</v>
+        <v>95</v>
+      </c>
+      <c r="D37" t="s">
+        <v>96</v>
       </c>
       <c r="E37" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F37">
         <v>1</v>
@@ -2241,319 +2223,319 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>149</v>
+        <v>97</v>
       </c>
       <c r="B38" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="C38" t="s">
-        <v>51</v>
+        <v>89</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>85</v>
+        <v>177</v>
       </c>
       <c r="E38" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F38">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>150</v>
+        <v>99</v>
       </c>
       <c r="B39" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="C39" t="s">
-        <v>51</v>
+        <v>89</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>86</v>
+        <v>178</v>
       </c>
       <c r="E39" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F39">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>151</v>
+        <v>101</v>
       </c>
       <c r="B40" t="s">
-        <v>87</v>
+        <v>102</v>
       </c>
       <c r="C40" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="E40" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F40">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
+        <v>103</v>
+      </c>
+      <c r="B41" t="s">
+        <v>104</v>
+      </c>
+      <c r="C41" t="s">
         <v>89</v>
       </c>
-      <c r="B41" t="s">
-        <v>90</v>
-      </c>
-      <c r="C41" t="s">
-        <v>88</v>
-      </c>
-      <c r="D41" t="s">
-        <v>91</v>
+      <c r="D41" s="2" t="s">
+        <v>180</v>
       </c>
       <c r="E41" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F41">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="B42" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="C42" t="s">
-        <v>94</v>
-      </c>
-      <c r="D42" t="s">
-        <v>95</v>
+        <v>89</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>176</v>
       </c>
       <c r="E42" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F42">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>152</v>
+        <v>107</v>
       </c>
       <c r="B43" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="C43" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="E43" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F43">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>97</v>
+        <v>108</v>
       </c>
       <c r="B44" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
       <c r="C44" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="E44" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F44">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>99</v>
+        <v>110</v>
       </c>
       <c r="B45" t="s">
-        <v>100</v>
+        <v>111</v>
       </c>
       <c r="C45" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="E45" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F45">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>153</v>
+        <v>112</v>
       </c>
       <c r="B46" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="C46" t="s">
-        <v>88</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>189</v>
+        <v>89</v>
+      </c>
+      <c r="D46" t="s">
+        <v>183</v>
       </c>
       <c r="E46" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F46">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>154</v>
+        <v>114</v>
       </c>
       <c r="B47" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C47" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="E47" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F47">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>155</v>
+        <v>115</v>
       </c>
       <c r="B48" t="s">
-        <v>101</v>
+        <v>116</v>
       </c>
       <c r="C48" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E48" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F48">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>156</v>
+        <v>117</v>
       </c>
       <c r="B49" t="s">
-        <v>103</v>
+        <v>118</v>
       </c>
       <c r="C49" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="E49" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F49">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>157</v>
+        <v>119</v>
       </c>
       <c r="B50" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
       <c r="C50" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="E50" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F50">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>105</v>
+        <v>121</v>
       </c>
       <c r="B51" t="s">
-        <v>106</v>
+        <v>122</v>
       </c>
       <c r="C51" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="E51" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F51">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>107</v>
+        <v>123</v>
       </c>
       <c r="B52" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="C52" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="E52" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F52">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>158</v>
+        <v>125</v>
       </c>
       <c r="B53" t="s">
-        <v>109</v>
+        <v>126</v>
       </c>
       <c r="C53" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="E53" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F53">
         <v>2</v>
@@ -2561,39 +2543,39 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>159</v>
+        <v>127</v>
       </c>
       <c r="B54" t="s">
-        <v>108</v>
+        <v>128</v>
       </c>
       <c r="C54" t="s">
-        <v>88</v>
+        <v>129</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>193</v>
+        <v>130</v>
       </c>
       <c r="E54" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F54">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>110</v>
+        <v>131</v>
       </c>
       <c r="B55" t="s">
-        <v>111</v>
+        <v>132</v>
       </c>
       <c r="C55" t="s">
-        <v>88</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>195</v>
+        <v>48</v>
+      </c>
+      <c r="D55" t="s">
+        <v>132</v>
       </c>
       <c r="E55" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F55">
         <v>1</v>
@@ -2601,59 +2583,59 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>160</v>
+        <v>133</v>
       </c>
       <c r="B56" t="s">
-        <v>106</v>
+        <v>134</v>
       </c>
       <c r="C56" t="s">
-        <v>88</v>
+        <v>135</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E56" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F56">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>161</v>
+        <v>136</v>
       </c>
       <c r="B57" t="s">
-        <v>112</v>
+        <v>137</v>
       </c>
       <c r="C57" t="s">
-        <v>88</v>
+        <v>138</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="E57" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F57">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>113</v>
+        <v>139</v>
       </c>
       <c r="B58" t="s">
-        <v>114</v>
+        <v>140</v>
       </c>
       <c r="C58" t="s">
-        <v>115</v>
+        <v>141</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>116</v>
+        <v>191</v>
       </c>
       <c r="E58" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F58">
         <v>1</v>
@@ -2661,19 +2643,19 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>117</v>
+        <v>142</v>
       </c>
       <c r="B59" t="s">
-        <v>118</v>
+        <v>143</v>
       </c>
       <c r="C59" t="s">
-        <v>41</v>
+        <v>144</v>
       </c>
       <c r="D59" t="s">
-        <v>118</v>
+        <v>192</v>
       </c>
       <c r="E59" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F59">
         <v>1</v>
@@ -2681,19 +2663,19 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>119</v>
+        <v>145</v>
       </c>
       <c r="B60" t="s">
-        <v>120</v>
+        <v>146</v>
       </c>
       <c r="C60" t="s">
-        <v>121</v>
+        <v>147</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>197</v>
+        <v>146</v>
       </c>
       <c r="E60" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F60">
         <v>1</v>
@@ -2701,19 +2683,19 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>122</v>
+        <v>148</v>
       </c>
       <c r="B61" t="s">
-        <v>123</v>
+        <v>149</v>
       </c>
       <c r="C61" t="s">
-        <v>124</v>
+        <v>150</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>123</v>
+        <v>193</v>
       </c>
       <c r="E61" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F61">
         <v>1</v>
@@ -2721,19 +2703,19 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>125</v>
+        <v>151</v>
       </c>
       <c r="B62" t="s">
-        <v>126</v>
+        <v>152</v>
       </c>
       <c r="C62" t="s">
-        <v>127</v>
+        <v>153</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="E62" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F62">
         <v>1</v>
@@ -2741,81 +2723,21 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>128</v>
+        <v>154</v>
       </c>
       <c r="B63" t="s">
-        <v>129</v>
+        <v>155</v>
       </c>
       <c r="C63" t="s">
-        <v>130</v>
+        <v>156</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>129</v>
+        <v>195</v>
       </c>
       <c r="E63" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F63">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
-        <v>131</v>
-      </c>
-      <c r="B64" t="s">
-        <v>132</v>
-      </c>
-      <c r="C64" t="s">
-        <v>133</v>
-      </c>
-      <c r="D64" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="E64" t="s">
-        <v>202</v>
-      </c>
-      <c r="F64">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
-        <v>134</v>
-      </c>
-      <c r="B65" t="s">
-        <v>135</v>
-      </c>
-      <c r="C65" t="s">
-        <v>136</v>
-      </c>
-      <c r="D65" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="E65" t="s">
-        <v>202</v>
-      </c>
-      <c r="F65">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
-        <v>137</v>
-      </c>
-      <c r="B66" t="s">
-        <v>138</v>
-      </c>
-      <c r="C66" t="s">
-        <v>139</v>
-      </c>
-      <c r="D66" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="E66" t="s">
-        <v>202</v>
-      </c>
-      <c r="F66">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
completed GPS ecoboda files
</commit_message>
<xml_diff>
--- a/BOM/GPS_MODULE_V3_BOM.xlsx
+++ b/BOM/GPS_MODULE_V3_BOM.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10" conformance="strict">
+<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\kicad6\KICAD 6.0.0\contractual_projects\ECO_BODA\GPS_BAORD\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{65DF5049-696E-4F7E-B13A-66B567588E1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{D1665FFF-4F14-44FE-AA38-BD991DC18048}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GPS_MODULE_V3.kicad_pro" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="313" uniqueCount="197">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="318" uniqueCount="200">
   <si>
     <t>Qty</t>
   </si>
@@ -42,9 +42,6 @@
     <t>MPN</t>
   </si>
   <si>
-    <t>AE1, AE2</t>
-  </si>
-  <si>
     <t>Antenna_Shield</t>
   </si>
   <si>
@@ -616,12 +613,24 @@
   </si>
   <si>
     <t>LCSC</t>
+  </si>
+  <si>
+    <t>AE2, AE3</t>
+  </si>
+  <si>
+    <t>AE1</t>
+  </si>
+  <si>
+    <t>Connector_Coaxial:SMA_Samtec_SMA-J-P-X-ST-EM1_EdgeMount</t>
+  </si>
+  <si>
+    <t>SMA-KE-347-H13.5-1.2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1105,12 +1114,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1465,11 +1475,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F63"/>
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D57" sqref="D57"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1495,67 +1505,67 @@
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="E2" t="s">
-        <v>196</v>
-      </c>
-      <c r="F2">
-        <v>2</v>
+      <c r="C2" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="F2" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>196</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>159</v>
+        <v>6</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>157</v>
       </c>
       <c r="E3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -1563,19 +1573,19 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -1583,179 +1593,179 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F6">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F8">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D9" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F9">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E10" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F10">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E11" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F11">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>168</v>
+        <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>29</v>
+        <v>166</v>
       </c>
       <c r="E12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F12">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>167</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C13" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="D13" t="s">
-        <v>167</v>
+        <v>28</v>
       </c>
       <c r="E13" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F13">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="C14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="E14" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F14">
         <v>3</v>
@@ -1763,39 +1773,39 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B15" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="E15" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F15">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B16" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="C16" t="s">
-        <v>36</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>35</v>
+        <v>12</v>
+      </c>
+      <c r="D16" t="s">
+        <v>168</v>
       </c>
       <c r="E16" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F16">
         <v>1</v>
@@ -1803,59 +1813,59 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B17" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C17" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E17" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F17">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C18" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>170</v>
+        <v>37</v>
       </c>
       <c r="E18" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F18">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C19" t="s">
-        <v>45</v>
-      </c>
-      <c r="D19" t="s">
-        <v>44</v>
+        <v>41</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>169</v>
       </c>
       <c r="E19" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F19">
         <v>1</v>
@@ -1863,19 +1873,19 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B20" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C20" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D20" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E20" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F20">
         <v>1</v>
@@ -1883,19 +1893,19 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B21" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C21" t="s">
-        <v>42</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>171</v>
+        <v>47</v>
+      </c>
+      <c r="D21" t="s">
+        <v>46</v>
       </c>
       <c r="E21" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F21">
         <v>1</v>
@@ -1903,19 +1913,19 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B22" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E22" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F22">
         <v>1</v>
@@ -1923,19 +1933,19 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B23" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C23" t="s">
-        <v>55</v>
-      </c>
-      <c r="D23" t="s">
-        <v>54</v>
+        <v>41</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>171</v>
       </c>
       <c r="E23" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F23">
         <v>1</v>
@@ -1943,59 +1953,59 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B24" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C24" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="D24" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E24" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F24">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B25" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C25" t="s">
-        <v>60</v>
-      </c>
-      <c r="D25" s="2">
-        <v>1751248</v>
+        <v>35</v>
+      </c>
+      <c r="D25" t="s">
+        <v>56</v>
       </c>
       <c r="E25" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F25">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B26" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C26" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D26" s="2">
-        <v>1053142204</v>
+        <v>1751248</v>
       </c>
       <c r="E26" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F26">
         <v>1</v>
@@ -2003,19 +2013,19 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B27" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C27" t="s">
-        <v>66</v>
-      </c>
-      <c r="D27" t="s">
-        <v>67</v>
+        <v>62</v>
+      </c>
+      <c r="D27" s="2">
+        <v>1053142204</v>
       </c>
       <c r="E27" t="s">
-        <v>173</v>
+        <v>195</v>
       </c>
       <c r="F27">
         <v>1</v>
@@ -2023,19 +2033,19 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B28" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C28" t="s">
-        <v>70</v>
-      </c>
-      <c r="D28">
-        <v>5033981892</v>
+        <v>65</v>
+      </c>
+      <c r="D28" t="s">
+        <v>66</v>
       </c>
       <c r="E28" t="s">
-        <v>196</v>
+        <v>172</v>
       </c>
       <c r="F28">
         <v>1</v>
@@ -2043,19 +2053,19 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B29" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C29" t="s">
-        <v>73</v>
-      </c>
-      <c r="D29" t="s">
-        <v>74</v>
+        <v>69</v>
+      </c>
+      <c r="D29">
+        <v>5033981892</v>
       </c>
       <c r="E29" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F29">
         <v>1</v>
@@ -2063,19 +2073,19 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B30" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C30" t="s">
-        <v>77</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>174</v>
+        <v>72</v>
+      </c>
+      <c r="D30" t="s">
+        <v>73</v>
       </c>
       <c r="E30" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F30">
         <v>1</v>
@@ -2083,19 +2093,19 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B31" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C31" t="s">
-        <v>80</v>
-      </c>
-      <c r="D31" t="s">
-        <v>175</v>
+        <v>76</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>173</v>
       </c>
       <c r="E31" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F31">
         <v>1</v>
@@ -2103,19 +2113,19 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B32" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C32" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="D32" t="s">
-        <v>82</v>
+        <v>174</v>
       </c>
       <c r="E32" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F32">
         <v>1</v>
@@ -2123,99 +2133,99 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B33" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C33" t="s">
-        <v>55</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>84</v>
+        <v>54</v>
+      </c>
+      <c r="D33" t="s">
+        <v>81</v>
       </c>
       <c r="E33" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F33">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B34" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C34" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E34" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F34">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B35" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C35" t="s">
-        <v>89</v>
+        <v>54</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>176</v>
+        <v>85</v>
       </c>
       <c r="E35" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F35">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B36" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C36" t="s">
-        <v>89</v>
-      </c>
-      <c r="D36" t="s">
-        <v>92</v>
+        <v>88</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>175</v>
       </c>
       <c r="E36" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F36">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B37" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C37" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="D37" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="E37" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F37">
         <v>1</v>
@@ -2223,59 +2233,59 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B38" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C38" t="s">
-        <v>89</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>177</v>
+        <v>94</v>
+      </c>
+      <c r="D38" t="s">
+        <v>95</v>
       </c>
       <c r="E38" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F38">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B39" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C39" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E39" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F39">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B40" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C40" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E40" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F40">
         <v>1</v>
@@ -2283,59 +2293,59 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B41" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C41" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E41" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F41">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B42" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C42" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="E42" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F42">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B43" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C43" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="E43" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F43">
         <v>3</v>
@@ -2343,79 +2353,79 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B44" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C44" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E44" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F44">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B45" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C45" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E45" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F45">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B46" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C46" t="s">
-        <v>89</v>
-      </c>
-      <c r="D46" t="s">
-        <v>183</v>
+        <v>88</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>181</v>
       </c>
       <c r="E46" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F46">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B47" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="C47" t="s">
-        <v>89</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>177</v>
+        <v>88</v>
+      </c>
+      <c r="D47" t="s">
+        <v>182</v>
       </c>
       <c r="E47" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F47">
         <v>1</v>
@@ -2423,39 +2433,39 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B48" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="C48" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="E48" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F48">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B49" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C49" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E49" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F49">
         <v>2</v>
@@ -2463,119 +2473,119 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B50" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C50" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E50" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F50">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B51" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C51" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E51" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F51">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B52" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C52" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="E52" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F52">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B53" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C53" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="E53" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F53">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B54" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C54" t="s">
-        <v>129</v>
+        <v>88</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>130</v>
+        <v>187</v>
       </c>
       <c r="E54" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F54">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B55" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="C55" t="s">
-        <v>48</v>
-      </c>
-      <c r="D55" t="s">
-        <v>132</v>
+        <v>128</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>129</v>
       </c>
       <c r="E55" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F55">
         <v>1</v>
@@ -2583,19 +2593,19 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B56" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C56" t="s">
-        <v>135</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>189</v>
+        <v>47</v>
+      </c>
+      <c r="D56" t="s">
+        <v>131</v>
       </c>
       <c r="E56" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F56">
         <v>1</v>
@@ -2603,19 +2613,19 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B57" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C57" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E57" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F57">
         <v>1</v>
@@ -2623,19 +2633,19 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B58" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C58" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E58" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F58">
         <v>1</v>
@@ -2643,19 +2653,19 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B59" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C59" t="s">
-        <v>144</v>
-      </c>
-      <c r="D59" t="s">
-        <v>192</v>
+        <v>140</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>190</v>
       </c>
       <c r="E59" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F59">
         <v>1</v>
@@ -2663,19 +2673,19 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B60" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C60" t="s">
-        <v>147</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
+      </c>
+      <c r="D60" t="s">
+        <v>191</v>
       </c>
       <c r="E60" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F60">
         <v>1</v>
@@ -2683,19 +2693,19 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B61" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C61" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>193</v>
+        <v>145</v>
       </c>
       <c r="E61" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F61">
         <v>1</v>
@@ -2703,19 +2713,19 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B62" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C62" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E62" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F62">
         <v>1</v>
@@ -2723,21 +2733,41 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
+        <v>150</v>
+      </c>
+      <c r="B63" t="s">
+        <v>151</v>
+      </c>
+      <c r="C63" t="s">
+        <v>152</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="E63" t="s">
+        <v>195</v>
+      </c>
+      <c r="F63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>153</v>
+      </c>
+      <c r="B64" t="s">
         <v>154</v>
       </c>
-      <c r="B63" t="s">
+      <c r="C64" t="s">
         <v>155</v>
       </c>
-      <c r="C63" t="s">
-        <v>156</v>
-      </c>
-      <c r="D63" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="E63" t="s">
-        <v>196</v>
-      </c>
-      <c r="F63">
+      <c r="D64" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="E64" t="s">
+        <v>195</v>
+      </c>
+      <c r="F64">
         <v>1</v>
       </c>
     </row>

</xml_diff>